<commit_message>
Reworked experiments figure to make them more readable. Also add baselines results to the feature transfer experiment on CoGenT.
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/cvpr_submission/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BDB21-F5FB-DB4A-B84D-B0071F1AA13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB48E04B-5EEE-0846-B0F9-C2B702A70020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">charts!$A$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">charts!$A$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">charts!$A$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">charts!$B$2:$F$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">charts!$B$3:$F$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">charts!$B$4:$F$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">charts!$B$5:$F$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +33,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
   <si>
     <t>Experiment</t>
   </si>
@@ -531,12 +542,6 @@
     <t>Finetune on CoGenT-B</t>
   </si>
   <si>
-    <t>CoGenT-A</t>
-  </si>
-  <si>
-    <t>CoGenT-B</t>
-  </si>
-  <si>
     <t>Finetuning on CoGenT-B (30k samples) for 1 epoch</t>
   </si>
   <si>
@@ -565,6 +570,30 @@
       </rPr>
       <t xml:space="preserve"> - 149,991 samples or heldout samples during finetuning - 119,961 samples)</t>
     </r>
+  </si>
+  <si>
+    <t>Test on CoGenT-A</t>
+  </si>
+  <si>
+    <t>Test on CoGenT-B</t>
+  </si>
+  <si>
+    <t>SAMNet</t>
+  </si>
+  <si>
+    <t>TbD (Paper)</t>
+  </si>
+  <si>
+    <t>PG + EE (Paper)</t>
+  </si>
+  <si>
+    <t>FiLM (Paper)</t>
+  </si>
+  <si>
+    <t>Zero-shot on CoGenT-B</t>
+  </si>
+  <si>
+    <t>Control on CoGenT-A</t>
   </si>
 </sst>
 </file>
@@ -825,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -907,6 +936,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,6 +982,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -994,19 +1031,9 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.23180686283849702"/>
-          <c:y val="3.5139983490663926E-2"/>
-          <c:w val="0.7169203128676378"/>
-          <c:h val="0.78092779701817405"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1042,13 +1069,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1070,15 +1097,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1182,39 +1200,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{12DF4109-83AB-5E41-948A-AE20B76B285B}" type="VALUE">
-                      <a:rPr lang="en-US" sz="1800"/>
-                      <a:pPr/>
-                      <a:t>[VALUE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="inEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-CDB5-CD4C-9297-8078B7AEC91C}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1223,13 +1208,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1360,13 +1345,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1461,13 +1446,13 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="50"/>
+        <c:gapWidth val="150"/>
         <c:axId val="556390528"/>
         <c:axId val="556419232"/>
       </c:barChart>
@@ -1477,7 +1462,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1530,7 +1515,7 @@
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1561,12 +1546,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1591,7 +1573,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1607,10 +1589,7 @@
           <a:pPr>
             <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1769,10 +1748,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>CoGenT-A</c:v>
+                  <c:v>Test on CoGenT-A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CoGenT-B</c:v>
+                  <c:v>Test on CoGenT-B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1890,10 +1869,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>CoGenT-A</c:v>
+                  <c:v>Test on CoGenT-A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CoGenT-B</c:v>
+                  <c:v>Test on CoGenT-B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2075,6 +2054,719 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.9718503745194477E-2"/>
+          <c:y val="7.9196212538971605E-2"/>
+          <c:w val="0.76780491488008862"/>
+          <c:h val="0.68823529635937442"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control on CoGenT-A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$15:$I$16</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SAMNet</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>TbD (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FiLM (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>PG + EE (Paper)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$17:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="0.0%">
+                  <c:v>0.95315611359999997</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0%">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0%">
+                  <c:v>0.98299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0%">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8D9-8B4F-A3AA-8536F5E70AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zero-shot on CoGenT-B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln w="3175">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$15:$I$16</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SAMNet</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>TbD (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FiLM (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>PG + EE (Paper)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>0.78220665450000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.754</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D8D9-8B4F-A3AA-8536F5E70AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Finetune on CoGenT-B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct5">
+              <a:fgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="dash"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$15:$I$16</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Test on CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Test on CoGenT-B</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SAMNet</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>TbD (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FiLM (Paper)</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>PG + EE (Paper)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$19:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.90806764360000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94026935099999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92700000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D8D9-8B4F-A3AA-8536F5E70AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="5"/>
+        <c:axId val="2064965920"/>
+        <c:axId val="2065156208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2064965920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2065156208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2065156208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.65000000000000013"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2064965920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83644357278305526"/>
+          <c:y val="0.2440545213633204"/>
+          <c:w val="0.16247658137471688"/>
+          <c:h val="0.48462095890719131"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -3189,16 +3881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>115558</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>43805</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>77753</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>147675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>387457</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>37345</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>540152</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>205304</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3225,16 +3917,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>699650</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171190</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1124066</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>21449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>91531</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>22884</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>363547</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>109421</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3254,6 +3946,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>614177</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>29534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>886045</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>177207</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4D40114-8959-4E45-A25F-9810E53323EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3594,44 +4322,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="41" t="s">
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="48"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="51"/>
     </row>
     <row r="2" spans="1:25" ht="20" thickBot="1">
-      <c r="A2" s="45"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
@@ -3804,7 +4532,7 @@
     </row>
     <row r="4" spans="1:25" ht="19">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
@@ -3884,7 +4612,7 @@
     </row>
     <row r="5" spans="1:25" ht="19">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
@@ -5112,36 +5840,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="13" style="26" customWidth="1"/>
-    <col min="3" max="3" width="12" style="26" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="26" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="26" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="26" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="26" customWidth="1"/>
     <col min="7" max="7" width="18" style="26" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="26"/>
+    <col min="8" max="8" width="20.33203125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="26" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="26" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="49" t="s">
+    <row r="1" spans="1:9">
+      <c r="B1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="31"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -5162,7 +5893,7 @@
       </c>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="27" t="s">
         <v>34</v>
       </c>
@@ -5188,7 +5919,7 @@
       </c>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="27" t="s">
         <v>32</v>
       </c>
@@ -5214,7 +5945,7 @@
       </c>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="27" t="s">
         <v>35</v>
       </c>
@@ -5240,24 +5971,24 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="52" t="s">
+    <row r="8" spans="1:9">
+      <c r="B8" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="56"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="32" t="s">
         <v>36</v>
       </c>
@@ -5270,7 +6001,7 @@
         <v>0.78220665450000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="32" t="s">
         <v>37</v>
       </c>
@@ -5283,10 +6014,220 @@
         <v>0.94026935099999998</v>
       </c>
     </row>
+    <row r="13" spans="1:9">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="30"/>
+      <c r="B15" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="52"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="30"/>
+      <c r="B16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="34">
+        <v>0.95315611359999997</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="34">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="34">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="G17" s="37"/>
+      <c r="H17" s="34">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0.78220665450000004</v>
+      </c>
+      <c r="E18" s="34">
+        <v>0.754</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="34">
+        <v>0.90806764360000003</v>
+      </c>
+      <c r="C19" s="34">
+        <v>0.94026935099999998</v>
+      </c>
+      <c r="D19" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E19" s="34">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="F19" s="34">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G19" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="H19" s="34">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finish standardizing experiments figures visual appearance.
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -8,23 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB48E04B-5EEE-0846-B0F9-C2B702A70020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BB2DE-8C58-8D43-9546-87E41392B57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">charts!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">charts!$A$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">charts!$A$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">charts!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">charts!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">charts!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">charts!$B$5:$F$5</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1069,7 +1060,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1190,7 +1181,9 @@
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="bg2"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -1208,7 +1201,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1345,7 +1338,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -2446,7 +2439,9 @@
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="bg2"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -5842,8 +5837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
Rewrite Experiments section and add back Summary.
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BB2DE-8C58-8D43-9546-87E41392B57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAE2A23-D7CD-234C-9017-A2122C2114B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
@@ -16,6 +16,11 @@
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">charts!$A$46</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">charts!$B$45:$D$45</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">charts!$B$46:$D$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>Experiment</t>
   </si>
@@ -585,6 +590,9 @@
   </si>
   <si>
     <t>Control on CoGenT-A</t>
+  </si>
+  <si>
+    <t>Accuracy on CLEVR</t>
   </si>
 </sst>
 </file>
@@ -2792,6 +2800,319 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy on CLEVR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>charts!$B$45:$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>SAMNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TbD (Paper)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FiLM (Paper)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PG + EE (Paper)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$46:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.96199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC95-CB46-BFBF-782568E92258}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1651611119"/>
+        <c:axId val="1651612751"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1651611119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1651612751"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1651612751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.84000000000000008"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1651611119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2.0000000000000004E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
@@ -2866,6 +3187,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3370,6 +3731,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3977,6 +4841,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>370840</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A76342BA-8547-1B4A-BD62-96BB2461A455}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5835,10 +6735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -6215,6 +7115,37 @@
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
     </row>
+    <row r="45" spans="1:7">
+      <c r="B45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="35">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="C46" s="35">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="D46" s="35">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E46" s="35">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F15:G15"/>

</xml_diff>

<commit_message>
Reworked Figure 1, 6.
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -8,18 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAE2A23-D7CD-234C-9017-A2122C2114B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1347C9C-ED5E-B947-982A-C8E2BCB90937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">charts!$A$46</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">charts!$B$45:$D$45</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">charts!$B$46:$D$46</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">charts!$A$63</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">charts!$A$64</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">charts!$B$62</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">charts!$B$63:$B$66</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">charts!$C$62</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">charts!$C$63:$C$66</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">charts!$D$62</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">charts!$D$63:$D$66</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">charts!$E$62</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">charts!$E$63:$E$66</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">charts!$A$65</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">charts!$A$66</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">charts!$B$62:$E$62</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">charts!$B$63:$E$63</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">charts!$B$64:$E$64</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">charts!$B$65:$E$65</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">charts!$B$66:$E$66</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">charts!$A$63:$A$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>Experiment</t>
   </si>
@@ -594,6 +609,21 @@
   <si>
     <t>Accuracy on CLEVR</t>
   </si>
+  <si>
+    <t>CoGenT-A  - CoGenT-A</t>
+  </si>
+  <si>
+    <t>CoGenT-B  - CoGenT-A
+(Fine-tuning)</t>
+  </si>
+  <si>
+    <t>CoGenT-A  - CoGenT-B
+(Zero-shot)</t>
+  </si>
+  <si>
+    <t>CoGenT-B  - CoGenT-B
+(Fine-tuning)</t>
+  </si>
 </sst>
 </file>
 
@@ -853,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -996,6 +1026,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2845,7 +2878,279 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltDnDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent4"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4347-E249-A2F9-E3F24AF2EB36}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="pct5">
+                <a:fgClr>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-4347-E249-A2F9-E3F24AF2EB36}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="lgGrid">
+                <a:fgClr>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent2"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-4347-E249-A2F9-E3F24AF2EB36}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-4347-E249-A2F9-E3F24AF2EB36}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4347-E249-A2F9-E3F24AF2EB36}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4347-E249-A2F9-E3F24AF2EB36}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4347-E249-A2F9-E3F24AF2EB36}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2886,10 +3191,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -3022,7 +3323,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.84000000000000008"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3071,7 +3372,7 @@
         <c:crossAx val="1651611119"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2.0000000000000004E-2"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3081,6 +3382,767 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10221241714620383"/>
+          <c:y val="4.484361994240392E-2"/>
+          <c:w val="0.88155381662002996"/>
+          <c:h val="0.66685307154984774"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SAMNet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>charts!$B$62:$E$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CoGenT-A  - CoGenT-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CoGenT-A  - CoGenT-B
+(Zero-shot)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CoGenT-B  - CoGenT-A
+(Fine-tuning)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CoGenT-B  - CoGenT-B
+(Fine-tuning)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$63:$E$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.95315611359999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-412D-A746-B0DC-F6E41F23A4BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PG + EE (Paper)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="lgGrid">
+              <a:fgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>charts!$B$62:$E$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CoGenT-A  - CoGenT-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CoGenT-A  - CoGenT-B
+(Zero-shot)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CoGenT-B  - CoGenT-A
+(Fine-tuning)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CoGenT-B  - CoGenT-B
+(Fine-tuning)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$64:$E$64</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92700000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-412D-A746-B0DC-F6E41F23A4BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FiLM (Paper)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct5">
+              <a:fgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>charts!$B$62:$E$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CoGenT-A  - CoGenT-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CoGenT-A  - CoGenT-B
+(Zero-shot)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CoGenT-B  - CoGenT-A
+(Fine-tuning)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CoGenT-B  - CoGenT-B
+(Fine-tuning)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$65:$E$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.98299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-412D-A746-B0DC-F6E41F23A4BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>charts!$A$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TbD (Paper)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>charts!$B$62:$E$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CoGenT-A  - CoGenT-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CoGenT-A  - CoGenT-B
+(Zero-shot)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CoGenT-B  - CoGenT-A
+(Fine-tuning)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CoGenT-B  - CoGenT-B
+(Fine-tuning)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>charts!$B$66:$E$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.754</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96299999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-412D-A746-B0DC-F6E41F23A4BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1894605727"/>
+        <c:axId val="1894737855"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1894605727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1894737855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1894737855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1894605727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27119011581435687"/>
+          <c:y val="0.91227252526863956"/>
+          <c:w val="0.54492823251305245"/>
+          <c:h val="8.7726543753240641E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4854,10 +5916,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1178560</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4877,6 +5939,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1595120</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>35560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10893CD2-F031-C74C-8360-90E5960A2871}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6735,19 +7833,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="26" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="26" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="26" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="24" style="26" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" style="26" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="26" customWidth="1"/>
     <col min="7" max="7" width="18" style="26" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" style="26" customWidth="1"/>
@@ -7146,8 +8244,224 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="30"/>
+      <c r="B56" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" s="52"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="30"/>
+      <c r="B57" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H57" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I57" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="34">
+        <v>0.95315611359999997</v>
+      </c>
+      <c r="C58" s="37"/>
+      <c r="D58" s="34">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E58" s="37"/>
+      <c r="F58" s="34">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="G58" s="37"/>
+      <c r="H58" s="34">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="I58" s="37"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="34">
+        <v>0.78220665450000004</v>
+      </c>
+      <c r="E59" s="34">
+        <v>0.754</v>
+      </c>
+      <c r="G59" s="34">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="I59" s="34">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="34">
+        <v>0.90806764360000003</v>
+      </c>
+      <c r="C60" s="34">
+        <v>0.94026935099999998</v>
+      </c>
+      <c r="D60" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E60" s="34">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="F60" s="34">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G60" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="H60" s="34">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="I60" s="34">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="40">
+      <c r="A62" s="30"/>
+      <c r="B62" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="34">
+        <v>0.95315611359999997</v>
+      </c>
+      <c r="C63" s="34">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D63" s="34">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="E63" s="34">
+        <v>0.94</v>
+      </c>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="34">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="C64" s="34">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D64" s="34">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="E64" s="34">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="34">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="C65" s="34">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="D65" s="34">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="E65" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="34">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="C66" s="34">
+        <v>0.754</v>
+      </c>
+      <c r="D66" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E66" s="34">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B1:F1"/>

</xml_diff>

<commit_message>
Reorganization and polishing of experimental plots
Signed-off-by: ibm <tkornuta.ibm@gmail.com>
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -5,37 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkornuta/Documents/git/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1347C9C-ED5E-B947-982A-C8E2BCB90937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C05B5EE-C00D-144E-B5F8-5D103CD051F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="3360" yWindow="480" windowWidth="21820" windowHeight="14460" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">charts!$A$63</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">charts!$A$64</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">charts!$B$62</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">charts!$B$63:$B$66</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">charts!$C$62</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">charts!$C$63:$C$66</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">charts!$D$62</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">charts!$D$63:$D$66</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">charts!$E$62</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">charts!$E$63:$E$66</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">charts!$A$65</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">charts!$A$66</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">charts!$B$62:$E$62</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">charts!$B$63:$E$63</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">charts!$B$64:$E$64</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">charts!$B$65:$E$65</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">charts!$B$66:$E$66</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">charts!$A$63:$A$66</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>Experiment</t>
   </si>
@@ -610,19 +590,31 @@
     <t>Accuracy on CLEVR</t>
   </si>
   <si>
-    <t>CoGenT-A  - CoGenT-A</t>
+    <t>CoGenT-A =&gt; CoGenT-A</t>
   </si>
   <si>
-    <t>CoGenT-B  - CoGenT-A
-(Fine-tuning)</t>
+    <t>CoGenT-A =&gt; CoGenT-B</t>
   </si>
   <si>
-    <t>CoGenT-A  - CoGenT-B
-(Zero-shot)</t>
+    <t>(Zero-shot)</t>
   </si>
   <si>
-    <t>CoGenT-B  - CoGenT-B
-(Fine-tuning)</t>
+    <t>(Fine-tuning on B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Compare
+Integer</t>
+  </si>
+  <si>
+    <t>Compare
+Attribute</t>
+  </si>
+  <si>
+    <t>Query
+Attribute</t>
   </si>
 </sst>
 </file>
@@ -883,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -970,6 +962,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,7 +1022,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1036,6 +1031,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBAECAC"/>
+      <color rgb="FF9DCDCF"/>
+      <color rgb="FFB790D2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1107,7 +1109,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1159,13 +1161,16 @@
                   <c:v>Count</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CompareInteger</c:v>
+                  <c:v>Compare
+Integer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CompareAttribute</c:v>
+                  <c:v>Compare
+Attribute</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>QueryAttribute</c:v>
+                  <c:v>Query
+Attribute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1218,12 +1223,13 @@
             <a:pattFill prst="pct5">
               <a:fgClr>
                 <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
                 </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
@@ -1248,7 +1254,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1300,13 +1306,16 @@
                   <c:v>Count</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CompareInteger</c:v>
+                  <c:v>Compare
+Integer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CompareAttribute</c:v>
+                  <c:v>Compare
+Attribute</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>QueryAttribute</c:v>
+                  <c:v>Query
+Attribute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1356,12 +1365,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="ltDnDiag">
+            <a:pattFill prst="wdDnDiag">
               <a:fgClr>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -1371,6 +1386,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3696233688898119E-3"/>
+                  <c:y val="-4.3721876546439428E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-B8F1-A74F-95ED-9E56E4AF56CA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1385,7 +1422,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1407,21 +1444,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -1437,13 +1460,16 @@
                   <c:v>Count</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CompareInteger</c:v>
+                  <c:v>Compare
+Integer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CompareAttribute</c:v>
+                  <c:v>Compare
+Attribute</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>QueryAttribute</c:v>
+                  <c:v>Query
+Attribute</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1486,7 +1512,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="50"/>
+        <c:overlap val="-10"/>
         <c:axId val="556390528"/>
         <c:axId val="556419232"/>
       </c:barChart>
@@ -1519,7 +1546,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="75000"/>
@@ -1596,7 +1623,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
-        <c:minorUnit val="5.000000000000001E-2"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1607,7 +1634,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1621,7 +1648,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -2883,14 +2910,14 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:pattFill prst="ltDnDiag">
+              <a:pattFill prst="lgGrid">
                 <a:fgClr>
-                  <a:schemeClr val="bg2">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:schemeClr val="accent4"/>
+                  <a:srgbClr val="BAECAC"/>
                 </a:bgClr>
               </a:pattFill>
               <a:ln>
@@ -2916,9 +2943,7 @@
                   </a:schemeClr>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="9DCDCF"/>
                 </a:bgClr>
               </a:pattFill>
               <a:ln>
@@ -2937,14 +2962,17 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:pattFill prst="lgGrid">
+              <a:pattFill prst="ltDnDiag">
                 <a:fgClr>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
                 </a:bgClr>
               </a:pattFill>
               <a:ln>
@@ -3219,13 +3247,13 @@
                   <c:v>SAMNet</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>TbD (Paper)</c:v>
+                  <c:v>PG + EE (Paper)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FiLM (Paper)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>PG + EE (Paper)</c:v>
+                  <c:v>TbD (Paper)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3240,13 +3268,13 @@
                   <c:v>0.96199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98699999999999999</c:v>
+                  <c:v>0.96899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.97699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96899999999999997</c:v>
+                  <c:v>0.98699999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3265,8 +3293,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="50"/>
         <c:axId val="1651611119"/>
         <c:axId val="1651612751"/>
       </c:barChart>
@@ -3323,7 +3350,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0"/>
+          <c:min val="0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3372,7 +3399,7 @@
         <c:crossAx val="1651611119"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.2"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3438,7 +3465,7 @@
           <c:x val="0.10221241714620383"/>
           <c:y val="4.484361994240392E-2"/>
           <c:w val="0.88155381662002996"/>
-          <c:h val="0.66685307154984774"/>
+          <c:h val="0.63113422145001619"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3450,7 +3477,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>charts!$A$63</c:f>
+              <c:f>charts!$A$65</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3478,13 +3505,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -3525,31 +3552,44 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>charts!$B$62:$E$62</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$63:$E$64</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>CoGenT-A  - CoGenT-A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CoGenT-A  - CoGenT-B
-(Zero-shot)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CoGenT-B  - CoGenT-A
-(Fine-tuning)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CoGenT-B  - CoGenT-B
-(Fine-tuning)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>  </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>(Zero-shot)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>charts!$B$63:$E$63</c:f>
+              <c:f>charts!$B$65:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3579,7 +3619,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>charts!$A$64</c:f>
+              <c:f>charts!$A$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3596,7 +3636,7 @@
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="BAECAC"/>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -3614,13 +3654,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3661,31 +3701,44 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>charts!$B$62:$E$62</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$63:$E$64</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>CoGenT-A  - CoGenT-A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CoGenT-A  - CoGenT-B
-(Zero-shot)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CoGenT-B  - CoGenT-A
-(Fine-tuning)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CoGenT-B  - CoGenT-B
-(Fine-tuning)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>  </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>(Zero-shot)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>charts!$B$64:$E$64</c:f>
+              <c:f>charts!$B$66:$E$66</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3715,7 +3768,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>charts!$A$65</c:f>
+              <c:f>charts!$A$67</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3732,9 +3785,7 @@
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
+                <a:srgbClr val="9DCDCF"/>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -3752,13 +3803,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3799,31 +3850,44 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>charts!$B$62:$E$62</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$63:$E$64</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>CoGenT-A  - CoGenT-A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CoGenT-A  - CoGenT-B
-(Zero-shot)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CoGenT-B  - CoGenT-A
-(Fine-tuning)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CoGenT-B  - CoGenT-B
-(Fine-tuning)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>  </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>(Zero-shot)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>charts!$B$65:$E$65</c:f>
+              <c:f>charts!$B$67:$E$67</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3853,7 +3917,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>charts!$A$66</c:f>
+              <c:f>charts!$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3870,7 +3934,10 @@
                 </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -3888,13 +3955,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3935,31 +4002,44 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>charts!$B$62:$E$62</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>charts!$B$63:$E$64</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>CoGenT-A  - CoGenT-A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CoGenT-A  - CoGenT-B
-(Zero-shot)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CoGenT-B  - CoGenT-A
-(Fine-tuning)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CoGenT-B  - CoGenT-B
-(Fine-tuning)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>  </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>(Zero-shot)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>(Fine-tuning on B)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>charts!$B$66:$E$66</c:f>
+              <c:f>charts!$B$68:$E$68</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3992,8 +4072,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="50"/>
+        <c:overlap val="-10"/>
         <c:axId val="1894605727"/>
         <c:axId val="1894737855"/>
       </c:barChart>
@@ -4012,7 +4092,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4023,7 +4103,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -4047,7 +4127,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.60000000000000009"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4096,6 +4176,7 @@
         <c:crossAx val="1894605727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4107,16 +4188,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.27119011581435687"/>
-          <c:y val="0.91227252526863956"/>
-          <c:w val="0.54492823251305245"/>
-          <c:h val="8.7726543753240641E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5805,13 +5876,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>77753</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>147675</xdr:rowOff>
+      <xdr:rowOff>147674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>540152</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>205304</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>145143</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>102420</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5910,16 +5981,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>370840</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1303901</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>127519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1178560</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>259183</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>173973</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5948,13 +6019,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1595120</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>35560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6283,8 +6354,8 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A35" sqref="A35"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6315,44 +6386,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="49" t="s">
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="52"/>
     </row>
     <row r="2" spans="1:25" ht="20" thickBot="1">
-      <c r="A2" s="48"/>
+      <c r="A2" s="49"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
@@ -7833,19 +7904,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="26" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="24" style="26" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="26" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="26" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="26" customWidth="1"/>
     <col min="7" max="7" width="18" style="26" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" style="26" customWidth="1"/>
@@ -7855,17 +7926,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="31"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="40">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -7875,14 +7946,14 @@
       <c r="C2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>6</v>
+      <c r="D2" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>57</v>
       </c>
       <c r="G2" s="29"/>
     </row>
@@ -7965,10 +8036,10 @@
       <c r="G5" s="30"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="56"/>
+      <c r="C8" s="57"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="32" t="s">
@@ -8019,22 +8090,22 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="30"/>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52" t="s">
+      <c r="E15" s="53"/>
+      <c r="F15" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52" t="s">
+      <c r="G15" s="53"/>
+      <c r="H15" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="52"/>
+      <c r="I15" s="53"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="30"/>
@@ -8218,13 +8289,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>46</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -8235,33 +8306,33 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="C46" s="35">
-        <v>0.98699999999999999</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="D46" s="35">
         <v>0.97699999999999998</v>
       </c>
       <c r="E46" s="35">
-        <v>0.96899999999999997</v>
+        <v>0.98699999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="30"/>
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52" t="s">
+      <c r="C56" s="53"/>
+      <c r="D56" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52" t="s">
+      <c r="E56" s="53"/>
+      <c r="F56" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52" t="s">
+      <c r="G56" s="53"/>
+      <c r="H56" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I56" s="52"/>
+      <c r="I56" s="53"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="30"/>
@@ -8357,61 +8428,38 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="40">
-      <c r="A62" s="30"/>
-      <c r="B62" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="57" t="s">
+    <row r="63" spans="1:9" ht="20">
+      <c r="A63" s="30"/>
+      <c r="B63" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D62" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62" s="57" t="s">
+      <c r="D63" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="34">
-        <v>0.95315611359999997</v>
-      </c>
-      <c r="C63" s="34">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="D63" s="34">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="E63" s="34">
-        <v>0.94</v>
+      <c r="E63" s="38" t="s">
+        <v>53</v>
       </c>
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B64" s="34">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="C64" s="34">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="D64" s="34">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="E64" s="34">
-        <v>0.92700000000000005</v>
+    <row r="64" spans="1:9" ht="19" customHeight="1">
+      <c r="A64" s="30"/>
+      <c r="B64" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="F64"/>
       <c r="G64"/>
@@ -8420,19 +8468,19 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B65" s="34">
-        <v>0.98299999999999998</v>
+        <v>0.95315611359999997</v>
       </c>
       <c r="C65" s="34">
-        <v>0.78800000000000003</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="D65" s="34">
-        <v>0.81100000000000005</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="E65" s="34">
-        <v>0.96899999999999997</v>
+        <v>0.94</v>
       </c>
       <c r="F65"/>
       <c r="G65"/>
@@ -8441,33 +8489,75 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B66" s="34">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="C66" s="34">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D66" s="34">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="E66" s="34">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="34">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="C67" s="34">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="D67" s="34">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="E67" s="34">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="34">
+      <c r="B68" s="34">
         <v>0.98799999999999999</v>
       </c>
-      <c r="C66" s="34">
+      <c r="C68" s="34">
         <v>0.754</v>
       </c>
-      <c r="D66" s="34">
+      <c r="D68" s="34">
         <v>0.96899999999999997</v>
       </c>
-      <c r="E66" s="34">
+      <c r="E68" s="34">
         <v>0.96299999999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Experiments: basics, feature transfer
Signed-off-by: ibm <tkornuta.ibm@gmail.com>
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkornuta/Documents/git/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C05B5EE-C00D-144E-B5F8-5D103CD051F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE871D9-C78B-D44F-93DF-4EDEDB6D17CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="480" windowWidth="21820" windowHeight="14460" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="3360" yWindow="460" windowWidth="21820" windowHeight="14460" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -965,6 +965,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,9 +1010,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,8 +1022,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3564,10 +3564,10 @@
                     <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3713,10 +3713,10 @@
                     <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3862,10 +3862,10 @@
                     <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -4014,10 +4014,10 @@
                     <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>CoGenT-A =&gt; CoGenT-A</c:v>
+                    <c:v>CoGenT-A =&gt; CoGenT-B</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -6386,44 +6386,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="45" t="s">
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="50" t="s">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="53"/>
     </row>
     <row r="2" spans="1:25" ht="20" thickBot="1">
-      <c r="A2" s="49"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
@@ -7906,8 +7906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -7946,13 +7946,13 @@
       <c r="C2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="39" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="29"/>
@@ -8090,22 +8090,22 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="30"/>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53" t="s">
+      <c r="C15" s="58"/>
+      <c r="D15" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53" t="s">
+      <c r="E15" s="58"/>
+      <c r="F15" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53" t="s">
+      <c r="G15" s="58"/>
+      <c r="H15" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="53"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="30"/>
@@ -8317,22 +8317,22 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="30"/>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53" t="s">
+      <c r="C56" s="58"/>
+      <c r="D56" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53" t="s">
+      <c r="E56" s="58"/>
+      <c r="F56" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53" t="s">
+      <c r="G56" s="58"/>
+      <c r="H56" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="I56" s="53"/>
+      <c r="I56" s="58"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="30"/>
@@ -8456,10 +8456,10 @@
         <v>51</v>
       </c>
       <c r="D64" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E64" s="38" t="s">
         <v>51</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>50</v>
       </c>
       <c r="F64"/>
       <c r="G64"/>
@@ -8548,6 +8548,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B15:C15"/>
@@ -8555,9 +8558,6 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Reduce font on some of the barcharts in Experiments section.
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/CLEVR_results.xlsx
+++ b/Transfer_Learning/results/CLEVR_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkornuta/Documents/git/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98744306-C300-C34C-A013-E398BDD67014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4560B605-4A97-DE47-AED4-7195925C3B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="460" windowWidth="21820" windowHeight="14460" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -1021,6 +1021,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1031,9 +1034,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1120,7 +1120,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1263,7 +1263,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1428,7 +1428,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2994,54 +2994,6 @@
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="bg1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="inEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="rect">
-                      <a:avLst/>
-                    </a:prstGeom>
-                  </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-4347-E249-A2F9-E3F24AF2EB36}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
               <c:idx val="1"/>
               <c:spPr>
                 <a:noFill/>
@@ -3057,7 +3009,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -3105,7 +3057,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -3153,7 +3105,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -3199,7 +3151,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -3517,7 +3469,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -3666,7 +3618,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3815,7 +3767,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3967,7 +3919,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -7912,8 +7864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1545FC5E-E989-1B4C-B489-41E1DEB5B90C}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="89" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -7932,13 +7884,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="31"/>
       <c r="H1" s="30"/>
     </row>
@@ -8042,10 +7994,10 @@
       <c r="G5" s="30"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="58"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="32" t="s">
@@ -8096,22 +8048,22 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="30"/>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58" t="s">
+      <c r="E15" s="54"/>
+      <c r="F15" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58" t="s">
+      <c r="G15" s="54"/>
+      <c r="H15" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="58"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="30"/>
@@ -8323,22 +8275,22 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="30"/>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58" t="s">
+      <c r="C56" s="54"/>
+      <c r="D56" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58" t="s">
+      <c r="E56" s="54"/>
+      <c r="F56" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58" t="s">
+      <c r="G56" s="54"/>
+      <c r="H56" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I56" s="58"/>
+      <c r="I56" s="54"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="30"/>

</xml_diff>